<commit_message>
Included movetoelement_click object type and included Tx and Support docs download objects.
</commit_message>
<xml_diff>
--- a/Fulcrum_PreProd_Trunk/src/com/proj/objectRepository/ObjectsFile_Transmittals.xlsx
+++ b/Fulcrum_PreProd_Trunk/src/com/proj/objectRepository/ObjectsFile_Transmittals.xlsx
@@ -5,7 +5,7 @@
   <workbookPr updateLinks="always"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\FluidTXGWS_Sprint5\Fulcrum_FluidTX_Trunk\src\com\proj\objectRepository\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\PreProdWS\Fulcrum_PreProd_Trunk\src\com\proj\objectRepository\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="238" uniqueCount="137">
   <si>
     <t>textbox</t>
   </si>
@@ -180,9 +180,6 @@
     <t>Tramsmittals-Contract</t>
   </si>
   <si>
-    <t>.//*[@id='DMSContractNumber_$containereditableRegion']</t>
-  </si>
-  <si>
     <t>Tramsmittals-Message</t>
   </si>
   <si>
@@ -204,9 +201,6 @@
     <t>Tramsmittals-TxType</t>
   </si>
   <si>
-    <t>.//*[@id='TransmittalType_$containereditableRegion']</t>
-  </si>
-  <si>
     <t>Tramsmittals-Complete Action</t>
   </si>
   <si>
@@ -270,18 +264,6 @@
     <t>.//*[text()='Forward']</t>
   </si>
   <si>
-    <t>Tramsmittals-Issue Reason</t>
-  </si>
-  <si>
-    <t>.//*[contains(@id,'IssueReason_')]</t>
-  </si>
-  <si>
-    <t>FluidTx component</t>
-  </si>
-  <si>
-    <t>Fulcrum Component</t>
-  </si>
-  <si>
     <t>Ribbon.Documents.New.AT.CompleteAction-Large</t>
   </si>
   <si>
@@ -439,6 +421,21 @@
   </si>
   <si>
     <t>button_scrollable</t>
+  </si>
+  <si>
+    <t>Tramsmittals- Response Required</t>
+  </si>
+  <si>
+    <t>.//*[contains(@id,'ResponseRequired_')]</t>
+  </si>
+  <si>
+    <t>Tramsmittals-View -Transmittal Files-Download</t>
+  </si>
+  <si>
+    <t>Tramsmittals-View -Supporting Document Files-Download</t>
+  </si>
+  <si>
+    <t>movetoelement_click</t>
   </si>
 </sst>
 </file>
@@ -482,7 +479,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -501,12 +498,6 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFFF00"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -522,7 +513,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
@@ -530,7 +521,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -880,10 +870,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A39"/>
+  <dimension ref="A2:A40"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="A40" sqref="A40:XFD40"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A41" sqref="A41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
@@ -1043,42 +1033,47 @@
     </row>
     <row r="32" spans="1:1">
       <c r="A32" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="33" spans="1:1">
       <c r="A33" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="34" spans="1:1">
       <c r="A34" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
     </row>
     <row r="35" spans="1:1">
       <c r="A35" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
     </row>
     <row r="36" spans="1:1">
       <c r="A36" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
     </row>
     <row r="37" spans="1:1">
       <c r="A37" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
     </row>
     <row r="38" spans="1:1">
       <c r="A38" t="s">
-        <v>129</v>
+        <v>123</v>
       </c>
     </row>
     <row r="39" spans="1:1">
       <c r="A39" t="s">
-        <v>137</v>
+        <v>131</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1">
+      <c r="A40" t="s">
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1095,11 +1090,9 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I53"/>
+  <dimension ref="A1:I39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -1134,19 +1127,19 @@
       </c>
     </row>
     <row r="2" spans="1:7">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="5" t="s">
         <v>34</v>
       </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:7">
       <c r="B3" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="C3" t="s">
         <v>35</v>
@@ -1155,7 +1148,7 @@
         <v>38</v>
       </c>
       <c r="E3" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
     </row>
     <row r="4" spans="1:7">
@@ -1216,56 +1209,49 @@
     </row>
     <row r="8" spans="1:7">
       <c r="B8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C8" t="s">
         <v>35</v>
       </c>
       <c r="D8" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E8" t="s">
-        <v>73</v>
-      </c>
-      <c r="G8" t="s">
-        <v>59</v>
+        <v>71</v>
       </c>
     </row>
     <row r="9" spans="1:7">
-      <c r="B9" s="5" t="s">
+      <c r="B9" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="C9" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D9" s="5" t="s">
-        <v>72</v>
-      </c>
-      <c r="E9" s="5" t="s">
-        <v>77</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5" t="s">
-        <v>84</v>
-      </c>
+      <c r="C9" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
     </row>
     <row r="10" spans="1:7">
-      <c r="B10" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="C10" s="5" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" s="5" t="s">
+      <c r="B10" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="D10" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="E10" s="5" t="s">
-        <v>82</v>
-      </c>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5" t="s">
-        <v>83</v>
-      </c>
+      <c r="E10" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
     </row>
     <row r="11" spans="1:7">
       <c r="B11" t="s">
@@ -1289,18 +1275,15 @@
         <v>35</v>
       </c>
       <c r="D12" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="E12" t="s">
-        <v>78</v>
-      </c>
-      <c r="G12" t="s">
-        <v>51</v>
+        <v>76</v>
       </c>
     </row>
     <row r="13" spans="1:7">
       <c r="B13" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
         <v>35</v>
@@ -1309,12 +1292,12 @@
         <v>0</v>
       </c>
       <c r="E13" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="14" spans="1:7">
       <c r="B14" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C14" t="s">
         <v>35</v>
@@ -1323,12 +1306,12 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="15" spans="1:7">
       <c r="B15" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C15" t="s">
         <v>35</v>
@@ -1337,12 +1320,12 @@
         <v>9</v>
       </c>
       <c r="E15" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="16" spans="1:7">
       <c r="B16" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="C16" t="s">
         <v>35</v>
@@ -1351,25 +1334,25 @@
         <v>9</v>
       </c>
       <c r="E16" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
     </row>
     <row r="17" spans="1:9">
-      <c r="A17" s="6" t="s">
-        <v>62</v>
-      </c>
-      <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
-      <c r="E17" s="6"/>
-      <c r="F17" s="6"/>
-      <c r="G17" s="6"/>
+      <c r="A17" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B17" s="5"/>
+      <c r="C17" s="5"/>
+      <c r="D17" s="5"/>
+      <c r="E17" s="5"/>
+      <c r="F17" s="5"/>
+      <c r="G17" s="5"/>
       <c r="H17" s="2"/>
       <c r="I17" s="2"/>
     </row>
     <row r="18" spans="1:9">
       <c r="B18" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C18" t="s">
         <v>35</v>
@@ -1378,12 +1361,12 @@
         <v>38</v>
       </c>
       <c r="E18" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="B19" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="C19" t="s">
         <v>35</v>
@@ -1392,12 +1375,12 @@
         <v>0</v>
       </c>
       <c r="E19" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="B20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="C20" t="s">
         <v>35</v>
@@ -1406,12 +1389,12 @@
         <v>23</v>
       </c>
       <c r="E20" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="B21" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="C21" t="s">
         <v>35</v>
@@ -1420,12 +1403,12 @@
         <v>9</v>
       </c>
       <c r="E21" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="B22" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
         <v>35</v>
@@ -1434,82 +1417,82 @@
         <v>21</v>
       </c>
       <c r="E22" t="s">
-        <v>106</v>
+        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="B23" t="s">
-        <v>108</v>
+        <v>134</v>
       </c>
       <c r="C23" t="s">
         <v>35</v>
       </c>
       <c r="D23" t="s">
-        <v>21</v>
+        <v>136</v>
       </c>
       <c r="E23" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="B24" t="s">
-        <v>117</v>
+        <v>102</v>
       </c>
       <c r="C24" t="s">
         <v>35</v>
       </c>
       <c r="D24" t="s">
-        <v>10</v>
+        <v>21</v>
       </c>
       <c r="E24" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="B25" t="s">
-        <v>112</v>
+        <v>135</v>
       </c>
       <c r="C25" t="s">
-        <v>86</v>
+        <v>35</v>
       </c>
       <c r="D25" t="s">
-        <v>9</v>
+        <v>136</v>
       </c>
       <c r="E25" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="B26" t="s">
-        <v>101</v>
+        <v>111</v>
       </c>
       <c r="C26" t="s">
         <v>35</v>
       </c>
       <c r="D26" t="s">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="E26" t="s">
-        <v>113</v>
+        <v>103</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="B27" t="s">
-        <v>98</v>
+        <v>106</v>
       </c>
       <c r="C27" t="s">
-        <v>35</v>
+        <v>80</v>
       </c>
       <c r="D27" t="s">
-        <v>21</v>
+        <v>9</v>
       </c>
       <c r="E27" t="s">
-        <v>97</v>
+        <v>105</v>
       </c>
     </row>
     <row r="28" spans="1:9">
       <c r="B28" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="C28" t="s">
         <v>35</v>
@@ -1518,26 +1501,26 @@
         <v>21</v>
       </c>
       <c r="E28" t="s">
-        <v>100</v>
+        <v>107</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="B29" t="s">
-        <v>130</v>
+        <v>92</v>
       </c>
       <c r="C29" t="s">
         <v>35</v>
       </c>
       <c r="D29" t="s">
-        <v>2</v>
+        <v>21</v>
       </c>
       <c r="E29" t="s">
-        <v>131</v>
+        <v>91</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="B30" t="s">
-        <v>133</v>
+        <v>93</v>
       </c>
       <c r="C30" t="s">
         <v>35</v>
@@ -1546,163 +1529,144 @@
         <v>21</v>
       </c>
       <c r="E30" t="s">
-        <v>134</v>
+        <v>94</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="B31" t="s">
-        <v>135</v>
+        <v>124</v>
       </c>
       <c r="C31" t="s">
         <v>35</v>
       </c>
       <c r="D31" t="s">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="E31" t="s">
-        <v>136</v>
+        <v>125</v>
       </c>
     </row>
     <row r="32" spans="1:9">
-      <c r="A32" s="6" t="s">
-        <v>114</v>
-      </c>
-      <c r="B32" s="6"/>
-      <c r="C32" s="6"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
+      <c r="B32" t="s">
+        <v>127</v>
+      </c>
+      <c r="C32" t="s">
+        <v>35</v>
+      </c>
+      <c r="D32" t="s">
+        <v>21</v>
+      </c>
+      <c r="E32" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="33" spans="1:7">
       <c r="B33" t="s">
-        <v>115</v>
+        <v>129</v>
       </c>
       <c r="C33" t="s">
         <v>35</v>
       </c>
       <c r="D33" t="s">
+        <v>8</v>
+      </c>
+      <c r="E33" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7">
+      <c r="A34" s="5" t="s">
+        <v>108</v>
+      </c>
+      <c r="B34" s="5"/>
+      <c r="C34" s="5"/>
+      <c r="D34" s="5"/>
+      <c r="E34" s="5"/>
+      <c r="F34" s="5"/>
+      <c r="G34" s="5"/>
+    </row>
+    <row r="35" spans="1:7">
+      <c r="B35" t="s">
+        <v>109</v>
+      </c>
+      <c r="C35" t="s">
+        <v>35</v>
+      </c>
+      <c r="D35" t="s">
         <v>21</v>
       </c>
-      <c r="E33" t="s">
+      <c r="E35" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="36" spans="1:7">
+      <c r="B36" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="34" spans="1:7">
-      <c r="B34" t="s">
-        <v>122</v>
-      </c>
-      <c r="C34" t="s">
-        <v>86</v>
-      </c>
-      <c r="D34" t="s">
-        <v>118</v>
-      </c>
-      <c r="E34" t="str">
+      <c r="C36" t="s">
+        <v>80</v>
+      </c>
+      <c r="D36" t="s">
+        <v>112</v>
+      </c>
+      <c r="E36" t="str">
         <f>Objects_Transmittals_Toolbar!E9</f>
         <v>Ribbon.ListForm.Display.Respond.Cancel-Medium</v>
       </c>
     </row>
-    <row r="35" spans="1:7">
-      <c r="B35" t="s">
+    <row r="37" spans="1:7">
+      <c r="B37" t="s">
+        <v>117</v>
+      </c>
+      <c r="C37" t="s">
+        <v>80</v>
+      </c>
+      <c r="D37" t="s">
         <v>123</v>
       </c>
-      <c r="C35" t="s">
-        <v>86</v>
-      </c>
-      <c r="D35" t="s">
-        <v>129</v>
-      </c>
-      <c r="E35" t="str">
-        <f>E34</f>
+      <c r="E37" t="str">
+        <f>E36</f>
         <v>Ribbon.ListForm.Display.Respond.Cancel-Medium</v>
       </c>
     </row>
-    <row r="36" spans="1:7">
-      <c r="B36" t="s">
-        <v>127</v>
-      </c>
-      <c r="C36" t="s">
-        <v>86</v>
-      </c>
-      <c r="D36" t="s">
-        <v>118</v>
-      </c>
-      <c r="E36" t="str">
+    <row r="38" spans="1:7">
+      <c r="B38" t="s">
+        <v>121</v>
+      </c>
+      <c r="C38" t="s">
+        <v>80</v>
+      </c>
+      <c r="D38" t="s">
+        <v>112</v>
+      </c>
+      <c r="E38" t="str">
         <f>Objects_Transmittals_Toolbar!E10</f>
         <v>Ribbon.Documents.New.AT.CloseTransmittal-Large</v>
       </c>
     </row>
-    <row r="37" spans="1:7">
-      <c r="B37" t="s">
-        <v>128</v>
-      </c>
-      <c r="C37" t="s">
-        <v>86</v>
-      </c>
-      <c r="D37" t="s">
-        <v>129</v>
-      </c>
-      <c r="E37" t="str">
-        <f>E36</f>
+    <row r="39" spans="1:7">
+      <c r="B39" t="s">
+        <v>122</v>
+      </c>
+      <c r="C39" t="s">
+        <v>80</v>
+      </c>
+      <c r="D39" t="s">
+        <v>123</v>
+      </c>
+      <c r="E39" t="str">
+        <f>E38</f>
         <v>Ribbon.Documents.New.AT.CloseTransmittal-Large</v>
       </c>
     </row>
-    <row r="42" spans="1:7">
-      <c r="E42" s="4"/>
-    </row>
-    <row r="43" spans="1:7">
-      <c r="E43" s="4"/>
-    </row>
-    <row r="44" spans="1:7">
-      <c r="E44" s="4"/>
-    </row>
-    <row r="45" spans="1:7">
-      <c r="E45" s="4"/>
-    </row>
-    <row r="47" spans="1:7">
-      <c r="A47" s="6"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="6"/>
-    </row>
-    <row r="49" spans="1:7">
-      <c r="A49" s="3"/>
-      <c r="F49" s="3"/>
-      <c r="G49" s="3"/>
-    </row>
-    <row r="50" spans="1:7">
-      <c r="A50" s="6"/>
-      <c r="B50" s="6"/>
-      <c r="C50" s="6"/>
-      <c r="D50" s="6"/>
-      <c r="E50" s="6"/>
-      <c r="F50" s="6"/>
-      <c r="G50" s="6"/>
-    </row>
-    <row r="53" spans="1:7">
-      <c r="A53" s="6"/>
-      <c r="B53" s="6"/>
-      <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
-      <c r="E53" s="6"/>
-      <c r="F53" s="6"/>
-      <c r="G53" s="6"/>
-    </row>
   </sheetData>
-  <mergeCells count="6">
+  <mergeCells count="3">
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A17:G17"/>
-    <mergeCell ref="A47:G47"/>
-    <mergeCell ref="A50:G50"/>
-    <mergeCell ref="A53:G53"/>
-    <mergeCell ref="A32:G32"/>
+    <mergeCell ref="A34:G34"/>
   </mergeCells>
   <dataValidations count="1">
-    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C51 C54 C3:C16 C48:C49 C33:C46 C18:C31">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="C35:C39 C18:C33 C3:C16">
       <formula1>"id,name,xpath"</formula1>
     </dataValidation>
   </dataValidations>
@@ -1711,48 +1675,12 @@
   <headerFooter alignWithMargins="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
-      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="7">
+      <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
         <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
           <x14:formula1>
             <xm:f>Objects!$A$2:$A$99</xm:f>
           </x14:formula1>
-          <xm:sqref>D46</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Objects!$A$2:$A$99</xm:f>
-          </x14:formula1>
-          <xm:sqref>D48:D49</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Objects!$A$2:$A$99</xm:f>
-          </x14:formula1>
-          <xm:sqref>D54</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Objects!$A$2:$A$99</xm:f>
-          </x14:formula1>
-          <xm:sqref>D51</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Objects!$A$2:$A$99</xm:f>
-          </x14:formula1>
-          <xm:sqref>D3:D16</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Objects!$A$2:$A$99</xm:f>
-          </x14:formula1>
-          <xm:sqref>D33:D37</xm:sqref>
-        </x14:dataValidation>
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
-          <x14:formula1>
-            <xm:f>Objects!$A$2:$A$99</xm:f>
-          </x14:formula1>
-          <xm:sqref>D18:D31</xm:sqref>
+          <xm:sqref>D35:D39 D18:D33 D3:D16</xm:sqref>
         </x14:dataValidation>
       </x14:dataValidations>
     </ext>
@@ -1764,9 +1692,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I44"/>
   <sheetViews>
-    <sheetView topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
   <cols>
@@ -1801,33 +1727,33 @@
       </c>
     </row>
     <row r="2" spans="1:9">
-      <c r="A2" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="B2" s="6"/>
-      <c r="C2" s="6"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="6"/>
-      <c r="F2" s="6"/>
-      <c r="G2" s="6"/>
+      <c r="A2" s="5" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="5"/>
+      <c r="C2" s="5"/>
+      <c r="D2" s="5"/>
+      <c r="E2" s="5"/>
+      <c r="F2" s="5"/>
+      <c r="G2" s="5"/>
     </row>
     <row r="3" spans="1:9">
       <c r="B3" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C3" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D3" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:9">
       <c r="B4" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C4" t="s">
         <v>35</v>
@@ -1836,137 +1762,137 @@
         <v>9</v>
       </c>
       <c r="E4" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
     </row>
     <row r="5" spans="1:9">
       <c r="B5" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D5" t="s">
         <v>12</v>
       </c>
       <c r="E5" t="s">
-        <v>104</v>
+        <v>98</v>
       </c>
     </row>
     <row r="6" spans="1:9">
       <c r="B6" t="s">
-        <v>88</v>
+        <v>82</v>
       </c>
       <c r="C6" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D6" t="s">
         <v>9</v>
       </c>
       <c r="E6" t="s">
-        <v>87</v>
+        <v>81</v>
       </c>
     </row>
     <row r="7" spans="1:9">
       <c r="B7" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="C7" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D7" t="s">
         <v>9</v>
       </c>
       <c r="E7" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="8" spans="1:9">
       <c r="B8" t="s">
-        <v>102</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D8" t="s">
         <v>9</v>
       </c>
       <c r="E8" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
     </row>
     <row r="9" spans="1:9">
       <c r="B9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C9" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D9" t="s">
         <v>9</v>
       </c>
       <c r="E9" t="s">
-        <v>124</v>
+        <v>118</v>
       </c>
     </row>
     <row r="10" spans="1:9">
       <c r="B10" t="s">
-        <v>126</v>
+        <v>120</v>
       </c>
       <c r="C10" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D10" t="s">
         <v>9</v>
       </c>
       <c r="E10" t="s">
-        <v>125</v>
+        <v>119</v>
       </c>
     </row>
     <row r="11" spans="1:9">
       <c r="B11" t="s">
-        <v>130</v>
+        <v>124</v>
       </c>
       <c r="C11" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
       <c r="D11" t="s">
         <v>9</v>
       </c>
       <c r="E11" t="s">
-        <v>132</v>
+        <v>126</v>
       </c>
     </row>
     <row r="12" spans="1:9">
-      <c r="A12" s="6" t="s">
-        <v>94</v>
-      </c>
-      <c r="B12" s="6"/>
-      <c r="C12" s="6"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
+      <c r="A12" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="B12" s="5"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
       <c r="H12" s="2"/>
       <c r="I12" s="2"/>
     </row>
     <row r="13" spans="1:9">
       <c r="B13" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="C13" t="s">
         <v>35</v>
       </c>
       <c r="D13" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
       <c r="E13" t="s">
-        <v>93</v>
+        <v>87</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="B14" t="s">
-        <v>95</v>
+        <v>89</v>
       </c>
       <c r="C14" t="s">
         <v>35</v>
@@ -1975,7 +1901,7 @@
         <v>9</v>
       </c>
       <c r="E14" t="s">
-        <v>96</v>
+        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:7">
@@ -1991,13 +1917,13 @@
       <c r="E36" s="4"/>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" s="6"/>
-      <c r="B38" s="6"/>
-      <c r="C38" s="6"/>
-      <c r="D38" s="6"/>
-      <c r="E38" s="6"/>
-      <c r="F38" s="6"/>
-      <c r="G38" s="6"/>
+      <c r="A38" s="5"/>
+      <c r="B38" s="5"/>
+      <c r="C38" s="5"/>
+      <c r="D38" s="5"/>
+      <c r="E38" s="5"/>
+      <c r="F38" s="5"/>
+      <c r="G38" s="5"/>
     </row>
     <row r="40" spans="1:7">
       <c r="A40" s="3"/>
@@ -2005,22 +1931,22 @@
       <c r="G40" s="3"/>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" s="6"/>
-      <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
-      <c r="D41" s="6"/>
-      <c r="E41" s="6"/>
-      <c r="F41" s="6"/>
-      <c r="G41" s="6"/>
+      <c r="A41" s="5"/>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="5"/>
+      <c r="F41" s="5"/>
+      <c r="G41" s="5"/>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" s="6"/>
-      <c r="B44" s="6"/>
-      <c r="C44" s="6"/>
-      <c r="D44" s="6"/>
-      <c r="E44" s="6"/>
-      <c r="F44" s="6"/>
-      <c r="G44" s="6"/>
+      <c r="A44" s="5"/>
+      <c r="B44" s="5"/>
+      <c r="C44" s="5"/>
+      <c r="D44" s="5"/>
+      <c r="E44" s="5"/>
+      <c r="F44" s="5"/>
+      <c r="G44" s="5"/>
     </row>
   </sheetData>
   <mergeCells count="5">

</xml_diff>